<commit_message>
Adding functionality for reading data from the documents, in progress
</commit_message>
<xml_diff>
--- a/data/zoo_data.xlsx
+++ b/data/zoo_data.xlsx
@@ -1,36 +1,150 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python learning\ZooManagementSystem\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="users" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="sections" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="cages" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="animals" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="users" sheetId="1" r:id="rId1"/>
+    <sheet name="sections" sheetId="2" r:id="rId2"/>
+    <sheet name="cages" sheetId="3" r:id="rId3"/>
+    <sheet name="animals" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>responsible_cages</t>
+  </si>
+  <si>
+    <t>shift_is_active</t>
+  </si>
+  <si>
+    <t>New owner name</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Maksym manager 1</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>Maksym manager 2</t>
+  </si>
+  <si>
+    <t>New user</t>
+  </si>
+  <si>
+    <t>cages</t>
+  </si>
+  <si>
+    <t>animals</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>animal_type</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>breed</t>
+  </si>
+  <si>
+    <t>fur_color</t>
+  </si>
+  <si>
+    <t>wing_span</t>
+  </si>
+  <si>
+    <t>can_fly</t>
+  </si>
+  <si>
+    <t>is_venomus</t>
+  </si>
+  <si>
+    <t>Section 1</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>Animal 1</t>
+  </si>
+  <si>
+    <t>reptile</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Animal 2</t>
+  </si>
+  <si>
+    <t>Animal 3</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>1;</t>
+  </si>
+  <si>
+    <t>2;3;</t>
+  </si>
+  <si>
+    <t>Section 2</t>
+  </si>
+  <si>
+    <t>Section 3</t>
+  </si>
+  <si>
+    <t>2;3;4;</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,80 +163,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -388,133 +443,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E4"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>role</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>responsible_cages</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>shift_is_active</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Maksym owner</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
       </c>
       <c r="E2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Maksym manager 1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>manager</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Maksym manager 2</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>manager</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>New user</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>manager</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -526,55 +543,187 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
First version of reading the data from the file
</commit_message>
<xml_diff>
--- a/data/zoo_data.xlsx
+++ b/data/zoo_data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
   <si>
     <t>id</t>
   </si>
@@ -45,9 +45,6 @@
     <t>owner</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Maksym manager 1</t>
   </si>
   <si>
@@ -63,9 +60,36 @@
     <t>cages</t>
   </si>
   <si>
+    <t>Section 1</t>
+  </si>
+  <si>
+    <t>1;</t>
+  </si>
+  <si>
+    <t>Section 2</t>
+  </si>
+  <si>
+    <t>Section 3</t>
+  </si>
+  <si>
+    <t>2;3;4;</t>
+  </si>
+  <si>
     <t>animals</t>
   </si>
   <si>
+    <t>1;2;3</t>
+  </si>
+  <si>
+    <t>4;6;</t>
+  </si>
+  <si>
+    <t>5;</t>
+  </si>
+  <si>
+    <t>7;8;</t>
+  </si>
+  <si>
     <t>age</t>
   </si>
   <si>
@@ -90,43 +114,82 @@
     <t>is_venomus</t>
   </si>
   <si>
-    <t>Section 1</t>
-  </si>
-  <si>
-    <t>1,2,3</t>
-  </si>
-  <si>
-    <t>Animal 1</t>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>mammal</t>
+  </si>
+  <si>
+    <t>Lion</t>
+  </si>
+  <si>
+    <t>African Lion</t>
+  </si>
+  <si>
+    <t>Golden</t>
+  </si>
+  <si>
+    <t>Molly</t>
+  </si>
+  <si>
+    <t>Dog</t>
+  </si>
+  <si>
+    <t>Labrador</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Snowy</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>British Shorthair</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Sky</t>
+  </si>
+  <si>
+    <t>bird</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Polly</t>
+  </si>
+  <si>
+    <t>Oscar</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Rex</t>
   </si>
   <si>
     <t>reptile</t>
   </si>
   <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>Animal 2</t>
-  </si>
-  <si>
-    <t>Animal 3</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>1;</t>
-  </si>
-  <si>
-    <t>2;3;</t>
-  </si>
-  <si>
-    <t>Section 2</t>
-  </si>
-  <si>
-    <t>Section 3</t>
-  </si>
-  <si>
-    <t>2;3;4;</t>
+    <t>Slither</t>
+  </si>
+  <si>
+    <t>Spike</t>
+  </si>
+  <si>
+    <t>1;4</t>
+  </si>
+  <si>
+    <t>3;</t>
+  </si>
+  <si>
+    <t>2;</t>
   </si>
 </sst>
 </file>
@@ -447,7 +510,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,9 +542,6 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
@@ -491,13 +551,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -508,13 +568,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -525,13 +585,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -560,7 +620,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -568,10 +628,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -579,7 +639,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -587,10 +647,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -600,10 +660,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -621,7 +681,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -631,10 +715,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,28 +731,28 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="J1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -676,16 +760,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -693,16 +783,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" t="s">
-        <v>26</v>
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -710,20 +806,137 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5">
+        <v>120</v>
+      </c>
+      <c r="I5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6">
+        <v>40</v>
+      </c>
+      <c r="I6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7">
+        <v>90</v>
+      </c>
+      <c r="I7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>